<commit_message>
modified:   python/or-tools/lot_size_problem_CP_SAT.py 	modified:   python/or-tools/production_results_ortools_CP.xlsx
</commit_message>
<xml_diff>
--- a/python/or-tools/production_results_ortools_CP.xlsx
+++ b/python/or-tools/production_results_ortools_CP.xlsx
@@ -808,7 +808,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="D22" t="n">
         <v>1</v>
@@ -825,13 +825,13 @@
         <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" t="n">
-        <v>300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -876,7 +876,7 @@
         <v>25</v>
       </c>
       <c r="C26" t="n">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="D26" t="n">
         <v>1</v>
@@ -893,13 +893,13 @@
         <v>26</v>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="D27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" t="n">
-        <v>300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -1352,7 +1352,7 @@
         <v>23</v>
       </c>
       <c r="C54" t="n">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="D54" t="n">
         <v>1</v>
@@ -1369,13 +1369,13 @@
         <v>24</v>
       </c>
       <c r="C55" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="D55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E55" t="n">
-        <v>300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -1403,7 +1403,7 @@
         <v>26</v>
       </c>
       <c r="C57" t="n">
-        <v>805</v>
+        <v>300</v>
       </c>
       <c r="D57" t="n">
         <v>1</v>
@@ -1420,13 +1420,13 @@
         <v>27</v>
       </c>
       <c r="C58" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="D58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E58" t="n">
-        <v>505</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59">
@@ -1437,13 +1437,13 @@
         <v>28</v>
       </c>
       <c r="C59" t="n">
-        <v>395</v>
+        <v>300</v>
       </c>
       <c r="D59" t="n">
         <v>1</v>
       </c>
       <c r="E59" t="n">
-        <v>205</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -1454,13 +1454,13 @@
         <v>29</v>
       </c>
       <c r="C60" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="D60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E60" t="n">
-        <v>300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -1474,7 +1474,7 @@
         <v>0</v>
       </c>
       <c r="D61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E61" t="n">
         <v>0</v>
@@ -1794,7 +1794,7 @@
         <v>19</v>
       </c>
       <c r="C80" t="n">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="D80" t="n">
         <v>1</v>
@@ -1811,13 +1811,13 @@
         <v>20</v>
       </c>
       <c r="C81" t="n">
-        <v>350</v>
+        <v>360</v>
       </c>
       <c r="D81" t="n">
         <v>1</v>
       </c>
       <c r="E81" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -1930,7 +1930,7 @@
         <v>27</v>
       </c>
       <c r="C88" t="n">
-        <v>720</v>
+        <v>360</v>
       </c>
       <c r="D88" t="n">
         <v>1</v>
@@ -1947,13 +1947,13 @@
         <v>28</v>
       </c>
       <c r="C89" t="n">
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="D89" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E89" t="n">
-        <v>360</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90">
@@ -1998,13 +1998,13 @@
         <v>1</v>
       </c>
       <c r="C92" t="n">
+        <v>0</v>
+      </c>
+      <c r="D92" t="n">
+        <v>0</v>
+      </c>
+      <c r="E92" t="n">
         <v>360</v>
-      </c>
-      <c r="D92" t="n">
-        <v>1</v>
-      </c>
-      <c r="E92" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="93">
@@ -2321,7 +2321,7 @@
         <v>20</v>
       </c>
       <c r="C111" t="n">
-        <v>472</v>
+        <v>360</v>
       </c>
       <c r="D111" t="n">
         <v>1</v>
@@ -2338,13 +2338,13 @@
         <v>21</v>
       </c>
       <c r="C112" t="n">
-        <v>248</v>
+        <v>360</v>
       </c>
       <c r="D112" t="n">
         <v>1</v>
       </c>
       <c r="E112" t="n">
-        <v>112</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113">
@@ -2355,7 +2355,7 @@
         <v>22</v>
       </c>
       <c r="C113" t="n">
-        <v>466</v>
+        <v>360</v>
       </c>
       <c r="D113" t="n">
         <v>1</v>
@@ -2372,13 +2372,13 @@
         <v>23</v>
       </c>
       <c r="C114" t="n">
-        <v>254</v>
+        <v>360</v>
       </c>
       <c r="D114" t="n">
         <v>1</v>
       </c>
       <c r="E114" t="n">
-        <v>106</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115">
@@ -2389,7 +2389,7 @@
         <v>24</v>
       </c>
       <c r="C115" t="n">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="D115" t="n">
         <v>1</v>
@@ -2406,13 +2406,13 @@
         <v>25</v>
       </c>
       <c r="C116" t="n">
-        <v>353</v>
+        <v>360</v>
       </c>
       <c r="D116" t="n">
         <v>1</v>
       </c>
       <c r="E116" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117">
@@ -2423,7 +2423,7 @@
         <v>26</v>
       </c>
       <c r="C117" t="n">
-        <v>897</v>
+        <v>360</v>
       </c>
       <c r="D117" t="n">
         <v>1</v>
@@ -2440,13 +2440,13 @@
         <v>27</v>
       </c>
       <c r="C118" t="n">
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="D118" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E118" t="n">
-        <v>537</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119">
@@ -2457,13 +2457,13 @@
         <v>28</v>
       </c>
       <c r="C119" t="n">
-        <v>183</v>
+        <v>360</v>
       </c>
       <c r="D119" t="n">
         <v>1</v>
       </c>
       <c r="E119" t="n">
-        <v>177</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120">
@@ -2508,13 +2508,13 @@
         <v>1</v>
       </c>
       <c r="C122" t="n">
-        <v>340</v>
+        <v>0</v>
       </c>
       <c r="D122" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E122" t="n">
-        <v>0</v>
+        <v>340</v>
       </c>
     </row>
     <row r="123">
@@ -2882,7 +2882,7 @@
         <v>23</v>
       </c>
       <c r="C144" t="n">
-        <v>680</v>
+        <v>340</v>
       </c>
       <c r="D144" t="n">
         <v>1</v>
@@ -2899,13 +2899,13 @@
         <v>24</v>
       </c>
       <c r="C145" t="n">
-        <v>0</v>
+        <v>340</v>
       </c>
       <c r="D145" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E145" t="n">
-        <v>340</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146">
@@ -2916,7 +2916,7 @@
         <v>25</v>
       </c>
       <c r="C146" t="n">
-        <v>368</v>
+        <v>340</v>
       </c>
       <c r="D146" t="n">
         <v>1</v>
@@ -2933,13 +2933,13 @@
         <v>26</v>
       </c>
       <c r="C147" t="n">
-        <v>652</v>
+        <v>340</v>
       </c>
       <c r="D147" t="n">
         <v>1</v>
       </c>
       <c r="E147" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148">
@@ -2950,13 +2950,13 @@
         <v>27</v>
       </c>
       <c r="C148" t="n">
-        <v>0</v>
+        <v>340</v>
       </c>
       <c r="D148" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E148" t="n">
-        <v>340</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149">
@@ -3018,13 +3018,13 @@
         <v>1</v>
       </c>
       <c r="C152" t="n">
-        <v>340</v>
+        <v>0</v>
       </c>
       <c r="D152" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E152" t="n">
-        <v>0</v>
+        <v>340</v>
       </c>
     </row>
     <row r="153">
@@ -3392,7 +3392,7 @@
         <v>23</v>
       </c>
       <c r="C174" t="n">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="D174" t="n">
         <v>1</v>
@@ -3409,13 +3409,13 @@
         <v>24</v>
       </c>
       <c r="C175" t="n">
-        <v>673</v>
+        <v>340</v>
       </c>
       <c r="D175" t="n">
         <v>1</v>
       </c>
       <c r="E175" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="176">
@@ -3426,13 +3426,13 @@
         <v>25</v>
       </c>
       <c r="C176" t="n">
-        <v>0</v>
+        <v>340</v>
       </c>
       <c r="D176" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E176" t="n">
-        <v>340</v>
+        <v>0</v>
       </c>
     </row>
     <row r="177">
@@ -3460,7 +3460,7 @@
         <v>27</v>
       </c>
       <c r="C178" t="n">
-        <v>680</v>
+        <v>340</v>
       </c>
       <c r="D178" t="n">
         <v>1</v>
@@ -3477,13 +3477,13 @@
         <v>28</v>
       </c>
       <c r="C179" t="n">
-        <v>0</v>
+        <v>340</v>
       </c>
       <c r="D179" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E179" t="n">
-        <v>340</v>
+        <v>0</v>
       </c>
     </row>
     <row r="180">
@@ -3514,7 +3514,7 @@
         <v>0</v>
       </c>
       <c r="D181" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E181" t="n">
         <v>0</v>
@@ -3936,7 +3936,7 @@
         <v>25</v>
       </c>
       <c r="C206" t="n">
-        <v>680</v>
+        <v>340</v>
       </c>
       <c r="D206" t="n">
         <v>1</v>
@@ -3953,13 +3953,13 @@
         <v>26</v>
       </c>
       <c r="C207" t="n">
-        <v>0</v>
+        <v>340</v>
       </c>
       <c r="D207" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E207" t="n">
-        <v>340</v>
+        <v>0</v>
       </c>
     </row>
     <row r="208">
@@ -3987,7 +3987,7 @@
         <v>28</v>
       </c>
       <c r="C209" t="n">
-        <v>900</v>
+        <v>340</v>
       </c>
       <c r="D209" t="n">
         <v>1</v>
@@ -4004,13 +4004,13 @@
         <v>29</v>
       </c>
       <c r="C210" t="n">
-        <v>1463</v>
+        <v>340</v>
       </c>
       <c r="D210" t="n">
         <v>1</v>
       </c>
       <c r="E210" t="n">
-        <v>560</v>
+        <v>0</v>
       </c>
     </row>
     <row r="211">
@@ -4024,10 +4024,10 @@
         <v>0</v>
       </c>
       <c r="D211" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E211" t="n">
-        <v>1683</v>
+        <v>0</v>
       </c>
     </row>
     <row r="212">
@@ -4038,13 +4038,13 @@
         <v>1</v>
       </c>
       <c r="C212" t="n">
-        <v>340</v>
+        <v>0</v>
       </c>
       <c r="D212" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E212" t="n">
-        <v>0</v>
+        <v>340</v>
       </c>
     </row>
     <row r="213">
@@ -4395,7 +4395,7 @@
         <v>22</v>
       </c>
       <c r="C233" t="n">
-        <v>680</v>
+        <v>340</v>
       </c>
       <c r="D233" t="n">
         <v>1</v>
@@ -4412,13 +4412,13 @@
         <v>23</v>
       </c>
       <c r="C234" t="n">
-        <v>0</v>
+        <v>340</v>
       </c>
       <c r="D234" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E234" t="n">
-        <v>340</v>
+        <v>0</v>
       </c>
     </row>
     <row r="235">
@@ -4429,7 +4429,7 @@
         <v>24</v>
       </c>
       <c r="C235" t="n">
-        <v>566</v>
+        <v>340</v>
       </c>
       <c r="D235" t="n">
         <v>1</v>
@@ -4446,13 +4446,13 @@
         <v>25</v>
       </c>
       <c r="C236" t="n">
-        <v>114</v>
+        <v>340</v>
       </c>
       <c r="D236" t="n">
         <v>1</v>
       </c>
       <c r="E236" t="n">
-        <v>226</v>
+        <v>0</v>
       </c>
     </row>
     <row r="237">
@@ -4480,7 +4480,7 @@
         <v>27</v>
       </c>
       <c r="C238" t="n">
-        <v>382</v>
+        <v>340</v>
       </c>
       <c r="D238" t="n">
         <v>1</v>
@@ -4497,13 +4497,13 @@
         <v>28</v>
       </c>
       <c r="C239" t="n">
-        <v>298</v>
+        <v>340</v>
       </c>
       <c r="D239" t="n">
         <v>1</v>
       </c>
       <c r="E239" t="n">
-        <v>42</v>
+        <v>0</v>
       </c>
     </row>
     <row r="240">
@@ -4548,13 +4548,13 @@
         <v>1</v>
       </c>
       <c r="C242" t="n">
+        <v>0</v>
+      </c>
+      <c r="D242" t="n">
+        <v>0</v>
+      </c>
+      <c r="E242" t="n">
         <v>208</v>
-      </c>
-      <c r="D242" t="n">
-        <v>1</v>
-      </c>
-      <c r="E242" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="243">
@@ -4582,7 +4582,7 @@
         <v>3</v>
       </c>
       <c r="C244" t="n">
-        <v>104</v>
+        <v>208</v>
       </c>
       <c r="D244" t="n">
         <v>1</v>
@@ -4599,13 +4599,13 @@
         <v>4</v>
       </c>
       <c r="C245" t="n">
-        <v>208</v>
+        <v>0</v>
       </c>
       <c r="D245" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E245" t="n">
-        <v>0</v>
+        <v>104</v>
       </c>
     </row>
     <row r="246">
@@ -4616,13 +4616,13 @@
         <v>5</v>
       </c>
       <c r="C246" t="n">
-        <v>0</v>
+        <v>208</v>
       </c>
       <c r="D246" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E246" t="n">
-        <v>104</v>
+        <v>0</v>
       </c>
     </row>
     <row r="247">
@@ -4633,13 +4633,13 @@
         <v>6</v>
       </c>
       <c r="C247" t="n">
+        <v>0</v>
+      </c>
+      <c r="D247" t="n">
+        <v>0</v>
+      </c>
+      <c r="E247" t="n">
         <v>104</v>
-      </c>
-      <c r="D247" t="n">
-        <v>1</v>
-      </c>
-      <c r="E247" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="248">
@@ -4650,7 +4650,7 @@
         <v>7</v>
       </c>
       <c r="C248" t="n">
-        <v>104</v>
+        <v>208</v>
       </c>
       <c r="D248" t="n">
         <v>1</v>
@@ -4667,13 +4667,13 @@
         <v>8</v>
       </c>
       <c r="C249" t="n">
-        <v>208</v>
+        <v>0</v>
       </c>
       <c r="D249" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E249" t="n">
-        <v>0</v>
+        <v>104</v>
       </c>
     </row>
     <row r="250">
@@ -4684,13 +4684,13 @@
         <v>9</v>
       </c>
       <c r="C250" t="n">
-        <v>0</v>
+        <v>208</v>
       </c>
       <c r="D250" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E250" t="n">
-        <v>104</v>
+        <v>0</v>
       </c>
     </row>
     <row r="251">
@@ -4701,13 +4701,13 @@
         <v>10</v>
       </c>
       <c r="C251" t="n">
-        <v>208</v>
+        <v>0</v>
       </c>
       <c r="D251" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E251" t="n">
-        <v>0</v>
+        <v>104</v>
       </c>
     </row>
     <row r="252">
@@ -4718,13 +4718,13 @@
         <v>11</v>
       </c>
       <c r="C252" t="n">
-        <v>0</v>
+        <v>208</v>
       </c>
       <c r="D252" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E252" t="n">
-        <v>104</v>
+        <v>0</v>
       </c>
     </row>
     <row r="253">
@@ -4735,13 +4735,13 @@
         <v>12</v>
       </c>
       <c r="C253" t="n">
+        <v>0</v>
+      </c>
+      <c r="D253" t="n">
+        <v>0</v>
+      </c>
+      <c r="E253" t="n">
         <v>104</v>
-      </c>
-      <c r="D253" t="n">
-        <v>1</v>
-      </c>
-      <c r="E253" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="254">
@@ -4786,7 +4786,7 @@
         <v>15</v>
       </c>
       <c r="C256" t="n">
-        <v>104</v>
+        <v>208</v>
       </c>
       <c r="D256" t="n">
         <v>1</v>
@@ -4803,13 +4803,13 @@
         <v>16</v>
       </c>
       <c r="C257" t="n">
+        <v>0</v>
+      </c>
+      <c r="D257" t="n">
+        <v>0</v>
+      </c>
+      <c r="E257" t="n">
         <v>104</v>
-      </c>
-      <c r="D257" t="n">
-        <v>1</v>
-      </c>
-      <c r="E257" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="258">
@@ -4854,7 +4854,7 @@
         <v>19</v>
       </c>
       <c r="C260" t="n">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="D260" t="n">
         <v>1</v>
@@ -4877,7 +4877,7 @@
         <v>0</v>
       </c>
       <c r="E261" t="n">
-        <v>117</v>
+        <v>104</v>
       </c>
     </row>
     <row r="262">
@@ -4888,13 +4888,13 @@
         <v>21</v>
       </c>
       <c r="C262" t="n">
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="D262" t="n">
         <v>1</v>
       </c>
       <c r="E262" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="263">
@@ -4990,7 +4990,7 @@
         <v>27</v>
       </c>
       <c r="C268" t="n">
-        <v>312</v>
+        <v>208</v>
       </c>
       <c r="D268" t="n">
         <v>1</v>
@@ -5013,7 +5013,7 @@
         <v>0</v>
       </c>
       <c r="E269" t="n">
-        <v>208</v>
+        <v>104</v>
       </c>
     </row>
     <row r="270">
@@ -5024,13 +5024,13 @@
         <v>29</v>
       </c>
       <c r="C270" t="n">
-        <v>0</v>
+        <v>104</v>
       </c>
       <c r="D270" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E270" t="n">
-        <v>104</v>
+        <v>0</v>
       </c>
     </row>
     <row r="271">
@@ -5044,7 +5044,7 @@
         <v>0</v>
       </c>
       <c r="D271" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E271" t="n">
         <v>0</v>
@@ -5058,13 +5058,13 @@
         <v>1</v>
       </c>
       <c r="C272" t="n">
+        <v>0</v>
+      </c>
+      <c r="D272" t="n">
+        <v>0</v>
+      </c>
+      <c r="E272" t="n">
         <v>138</v>
-      </c>
-      <c r="D272" t="n">
-        <v>1</v>
-      </c>
-      <c r="E272" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="273">
@@ -5092,7 +5092,7 @@
         <v>3</v>
       </c>
       <c r="C274" t="n">
-        <v>138</v>
+        <v>207</v>
       </c>
       <c r="D274" t="n">
         <v>1</v>
@@ -5115,7 +5115,7 @@
         <v>0</v>
       </c>
       <c r="E275" t="n">
-        <v>69</v>
+        <v>138</v>
       </c>
     </row>
     <row r="276">
@@ -5126,13 +5126,13 @@
         <v>5</v>
       </c>
       <c r="C276" t="n">
-        <v>138</v>
+        <v>0</v>
       </c>
       <c r="D276" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E276" t="n">
-        <v>0</v>
+        <v>69</v>
       </c>
     </row>
     <row r="277">
@@ -5143,13 +5143,13 @@
         <v>6</v>
       </c>
       <c r="C277" t="n">
-        <v>0</v>
+        <v>207</v>
       </c>
       <c r="D277" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E277" t="n">
-        <v>69</v>
+        <v>0</v>
       </c>
     </row>
     <row r="278">
@@ -5160,13 +5160,13 @@
         <v>7</v>
       </c>
       <c r="C278" t="n">
+        <v>0</v>
+      </c>
+      <c r="D278" t="n">
+        <v>0</v>
+      </c>
+      <c r="E278" t="n">
         <v>138</v>
-      </c>
-      <c r="D278" t="n">
-        <v>1</v>
-      </c>
-      <c r="E278" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="279">
@@ -5194,7 +5194,7 @@
         <v>9</v>
       </c>
       <c r="C280" t="n">
-        <v>138</v>
+        <v>207</v>
       </c>
       <c r="D280" t="n">
         <v>1</v>
@@ -5217,7 +5217,7 @@
         <v>0</v>
       </c>
       <c r="E281" t="n">
-        <v>69</v>
+        <v>138</v>
       </c>
     </row>
     <row r="282">
@@ -5228,13 +5228,13 @@
         <v>11</v>
       </c>
       <c r="C282" t="n">
-        <v>138</v>
+        <v>0</v>
       </c>
       <c r="D282" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E282" t="n">
-        <v>0</v>
+        <v>69</v>
       </c>
     </row>
     <row r="283">
@@ -5245,13 +5245,13 @@
         <v>12</v>
       </c>
       <c r="C283" t="n">
-        <v>0</v>
+        <v>207</v>
       </c>
       <c r="D283" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E283" t="n">
-        <v>69</v>
+        <v>0</v>
       </c>
     </row>
     <row r="284">
@@ -5262,13 +5262,13 @@
         <v>13</v>
       </c>
       <c r="C284" t="n">
+        <v>0</v>
+      </c>
+      <c r="D284" t="n">
+        <v>0</v>
+      </c>
+      <c r="E284" t="n">
         <v>138</v>
-      </c>
-      <c r="D284" t="n">
-        <v>1</v>
-      </c>
-      <c r="E284" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="285">
@@ -5296,7 +5296,7 @@
         <v>15</v>
       </c>
       <c r="C286" t="n">
-        <v>138</v>
+        <v>207</v>
       </c>
       <c r="D286" t="n">
         <v>1</v>
@@ -5319,7 +5319,7 @@
         <v>0</v>
       </c>
       <c r="E287" t="n">
-        <v>69</v>
+        <v>138</v>
       </c>
     </row>
     <row r="288">
@@ -5330,13 +5330,13 @@
         <v>17</v>
       </c>
       <c r="C288" t="n">
-        <v>138</v>
+        <v>0</v>
       </c>
       <c r="D288" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E288" t="n">
-        <v>0</v>
+        <v>69</v>
       </c>
     </row>
     <row r="289">
@@ -5347,13 +5347,13 @@
         <v>18</v>
       </c>
       <c r="C289" t="n">
-        <v>0</v>
+        <v>207</v>
       </c>
       <c r="D289" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E289" t="n">
-        <v>69</v>
+        <v>0</v>
       </c>
     </row>
     <row r="290">
@@ -5364,13 +5364,13 @@
         <v>19</v>
       </c>
       <c r="C290" t="n">
+        <v>0</v>
+      </c>
+      <c r="D290" t="n">
+        <v>0</v>
+      </c>
+      <c r="E290" t="n">
         <v>138</v>
-      </c>
-      <c r="D290" t="n">
-        <v>1</v>
-      </c>
-      <c r="E290" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="291">
@@ -5500,7 +5500,7 @@
         <v>27</v>
       </c>
       <c r="C298" t="n">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="D298" t="n">
         <v>1</v>
@@ -5517,13 +5517,13 @@
         <v>28</v>
       </c>
       <c r="C299" t="n">
-        <v>1087</v>
+        <v>0</v>
       </c>
       <c r="D299" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E299" t="n">
-        <v>0</v>
+        <v>138</v>
       </c>
     </row>
     <row r="300">
@@ -5540,7 +5540,7 @@
         <v>0</v>
       </c>
       <c r="E300" t="n">
-        <v>1018</v>
+        <v>69</v>
       </c>
     </row>
     <row r="301">
@@ -5557,7 +5557,7 @@
         <v>1</v>
       </c>
       <c r="E301" t="n">
-        <v>949</v>
+        <v>0</v>
       </c>
     </row>
     <row r="302">
@@ -5568,13 +5568,13 @@
         <v>1</v>
       </c>
       <c r="C302" t="n">
+        <v>0</v>
+      </c>
+      <c r="D302" t="n">
+        <v>0</v>
+      </c>
+      <c r="E302" t="n">
         <v>114</v>
-      </c>
-      <c r="D302" t="n">
-        <v>1</v>
-      </c>
-      <c r="E302" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="303">
@@ -5585,7 +5585,7 @@
         <v>2</v>
       </c>
       <c r="C303" t="n">
-        <v>114</v>
+        <v>228</v>
       </c>
       <c r="D303" t="n">
         <v>1</v>
@@ -5602,13 +5602,13 @@
         <v>3</v>
       </c>
       <c r="C304" t="n">
+        <v>0</v>
+      </c>
+      <c r="D304" t="n">
+        <v>0</v>
+      </c>
+      <c r="E304" t="n">
         <v>114</v>
-      </c>
-      <c r="D304" t="n">
-        <v>1</v>
-      </c>
-      <c r="E304" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="305">
@@ -5619,7 +5619,7 @@
         <v>4</v>
       </c>
       <c r="C305" t="n">
-        <v>114</v>
+        <v>228</v>
       </c>
       <c r="D305" t="n">
         <v>1</v>
@@ -5636,13 +5636,13 @@
         <v>5</v>
       </c>
       <c r="C306" t="n">
+        <v>0</v>
+      </c>
+      <c r="D306" t="n">
+        <v>0</v>
+      </c>
+      <c r="E306" t="n">
         <v>114</v>
-      </c>
-      <c r="D306" t="n">
-        <v>1</v>
-      </c>
-      <c r="E306" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="307">
@@ -5653,7 +5653,7 @@
         <v>6</v>
       </c>
       <c r="C307" t="n">
-        <v>114</v>
+        <v>228</v>
       </c>
       <c r="D307" t="n">
         <v>1</v>
@@ -5670,13 +5670,13 @@
         <v>7</v>
       </c>
       <c r="C308" t="n">
+        <v>0</v>
+      </c>
+      <c r="D308" t="n">
+        <v>0</v>
+      </c>
+      <c r="E308" t="n">
         <v>114</v>
-      </c>
-      <c r="D308" t="n">
-        <v>1</v>
-      </c>
-      <c r="E308" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="309">
@@ -5687,7 +5687,7 @@
         <v>8</v>
       </c>
       <c r="C309" t="n">
-        <v>114</v>
+        <v>228</v>
       </c>
       <c r="D309" t="n">
         <v>1</v>
@@ -5704,13 +5704,13 @@
         <v>9</v>
       </c>
       <c r="C310" t="n">
+        <v>0</v>
+      </c>
+      <c r="D310" t="n">
+        <v>0</v>
+      </c>
+      <c r="E310" t="n">
         <v>114</v>
-      </c>
-      <c r="D310" t="n">
-        <v>1</v>
-      </c>
-      <c r="E310" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="311">
@@ -5721,7 +5721,7 @@
         <v>10</v>
       </c>
       <c r="C311" t="n">
-        <v>114</v>
+        <v>228</v>
       </c>
       <c r="D311" t="n">
         <v>1</v>
@@ -5738,13 +5738,13 @@
         <v>11</v>
       </c>
       <c r="C312" t="n">
+        <v>0</v>
+      </c>
+      <c r="D312" t="n">
+        <v>0</v>
+      </c>
+      <c r="E312" t="n">
         <v>114</v>
-      </c>
-      <c r="D312" t="n">
-        <v>1</v>
-      </c>
-      <c r="E312" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="313">
@@ -5755,7 +5755,7 @@
         <v>12</v>
       </c>
       <c r="C313" t="n">
-        <v>114</v>
+        <v>228</v>
       </c>
       <c r="D313" t="n">
         <v>1</v>
@@ -5772,13 +5772,13 @@
         <v>13</v>
       </c>
       <c r="C314" t="n">
+        <v>0</v>
+      </c>
+      <c r="D314" t="n">
+        <v>0</v>
+      </c>
+      <c r="E314" t="n">
         <v>114</v>
-      </c>
-      <c r="D314" t="n">
-        <v>1</v>
-      </c>
-      <c r="E314" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="315">
@@ -5789,7 +5789,7 @@
         <v>14</v>
       </c>
       <c r="C315" t="n">
-        <v>114</v>
+        <v>228</v>
       </c>
       <c r="D315" t="n">
         <v>1</v>
@@ -5806,13 +5806,13 @@
         <v>15</v>
       </c>
       <c r="C316" t="n">
+        <v>0</v>
+      </c>
+      <c r="D316" t="n">
+        <v>0</v>
+      </c>
+      <c r="E316" t="n">
         <v>114</v>
-      </c>
-      <c r="D316" t="n">
-        <v>1</v>
-      </c>
-      <c r="E316" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="317">
@@ -5823,7 +5823,7 @@
         <v>16</v>
       </c>
       <c r="C317" t="n">
-        <v>114</v>
+        <v>228</v>
       </c>
       <c r="D317" t="n">
         <v>1</v>
@@ -5840,13 +5840,13 @@
         <v>17</v>
       </c>
       <c r="C318" t="n">
-        <v>228</v>
+        <v>0</v>
       </c>
       <c r="D318" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E318" t="n">
-        <v>0</v>
+        <v>114</v>
       </c>
     </row>
     <row r="319">
@@ -5857,13 +5857,13 @@
         <v>18</v>
       </c>
       <c r="C319" t="n">
-        <v>0</v>
+        <v>228</v>
       </c>
       <c r="D319" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E319" t="n">
-        <v>114</v>
+        <v>0</v>
       </c>
     </row>
     <row r="320">
@@ -5874,13 +5874,13 @@
         <v>19</v>
       </c>
       <c r="C320" t="n">
-        <v>228</v>
+        <v>0</v>
       </c>
       <c r="D320" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E320" t="n">
-        <v>0</v>
+        <v>114</v>
       </c>
     </row>
     <row r="321">
@@ -5891,13 +5891,13 @@
         <v>20</v>
       </c>
       <c r="C321" t="n">
-        <v>0</v>
+        <v>228</v>
       </c>
       <c r="D321" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E321" t="n">
-        <v>114</v>
+        <v>0</v>
       </c>
     </row>
     <row r="322">
@@ -5908,13 +5908,13 @@
         <v>21</v>
       </c>
       <c r="C322" t="n">
-        <v>228</v>
+        <v>0</v>
       </c>
       <c r="D322" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E322" t="n">
-        <v>0</v>
+        <v>114</v>
       </c>
     </row>
     <row r="323">
@@ -5925,13 +5925,13 @@
         <v>22</v>
       </c>
       <c r="C323" t="n">
-        <v>0</v>
+        <v>228</v>
       </c>
       <c r="D323" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E323" t="n">
-        <v>114</v>
+        <v>0</v>
       </c>
     </row>
     <row r="324">
@@ -5942,13 +5942,13 @@
         <v>23</v>
       </c>
       <c r="C324" t="n">
-        <v>228</v>
+        <v>0</v>
       </c>
       <c r="D324" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E324" t="n">
-        <v>0</v>
+        <v>114</v>
       </c>
     </row>
     <row r="325">
@@ -5959,13 +5959,13 @@
         <v>24</v>
       </c>
       <c r="C325" t="n">
-        <v>0</v>
+        <v>228</v>
       </c>
       <c r="D325" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E325" t="n">
-        <v>114</v>
+        <v>0</v>
       </c>
     </row>
     <row r="326">
@@ -5976,13 +5976,13 @@
         <v>25</v>
       </c>
       <c r="C326" t="n">
+        <v>0</v>
+      </c>
+      <c r="D326" t="n">
+        <v>0</v>
+      </c>
+      <c r="E326" t="n">
         <v>114</v>
-      </c>
-      <c r="D326" t="n">
-        <v>1</v>
-      </c>
-      <c r="E326" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="327">
@@ -6027,7 +6027,7 @@
         <v>28</v>
       </c>
       <c r="C329" t="n">
-        <v>114</v>
+        <v>228</v>
       </c>
       <c r="D329" t="n">
         <v>1</v>
@@ -6044,13 +6044,13 @@
         <v>29</v>
       </c>
       <c r="C330" t="n">
+        <v>0</v>
+      </c>
+      <c r="D330" t="n">
+        <v>0</v>
+      </c>
+      <c r="E330" t="n">
         <v>114</v>
-      </c>
-      <c r="D330" t="n">
-        <v>1</v>
-      </c>
-      <c r="E330" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="331">
@@ -6064,7 +6064,7 @@
         <v>0</v>
       </c>
       <c r="D331" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E331" t="n">
         <v>0</v>
@@ -6078,13 +6078,13 @@
         <v>1</v>
       </c>
       <c r="C332" t="n">
+        <v>0</v>
+      </c>
+      <c r="D332" t="n">
+        <v>0</v>
+      </c>
+      <c r="E332" t="n">
         <v>208</v>
-      </c>
-      <c r="D332" t="n">
-        <v>1</v>
-      </c>
-      <c r="E332" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="333">
@@ -6112,7 +6112,7 @@
         <v>3</v>
       </c>
       <c r="C334" t="n">
-        <v>104</v>
+        <v>208</v>
       </c>
       <c r="D334" t="n">
         <v>1</v>
@@ -6129,13 +6129,13 @@
         <v>4</v>
       </c>
       <c r="C335" t="n">
+        <v>0</v>
+      </c>
+      <c r="D335" t="n">
+        <v>0</v>
+      </c>
+      <c r="E335" t="n">
         <v>104</v>
-      </c>
-      <c r="D335" t="n">
-        <v>1</v>
-      </c>
-      <c r="E335" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="336">
@@ -6214,7 +6214,7 @@
         <v>9</v>
       </c>
       <c r="C340" t="n">
-        <v>104</v>
+        <v>208</v>
       </c>
       <c r="D340" t="n">
         <v>1</v>
@@ -6231,13 +6231,13 @@
         <v>10</v>
       </c>
       <c r="C341" t="n">
+        <v>0</v>
+      </c>
+      <c r="D341" t="n">
+        <v>0</v>
+      </c>
+      <c r="E341" t="n">
         <v>104</v>
-      </c>
-      <c r="D341" t="n">
-        <v>1</v>
-      </c>
-      <c r="E341" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="342">
@@ -6282,7 +6282,7 @@
         <v>13</v>
       </c>
       <c r="C344" t="n">
-        <v>104</v>
+        <v>208</v>
       </c>
       <c r="D344" t="n">
         <v>1</v>
@@ -6299,13 +6299,13 @@
         <v>14</v>
       </c>
       <c r="C345" t="n">
-        <v>208</v>
+        <v>0</v>
       </c>
       <c r="D345" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E345" t="n">
-        <v>0</v>
+        <v>104</v>
       </c>
     </row>
     <row r="346">
@@ -6316,13 +6316,13 @@
         <v>15</v>
       </c>
       <c r="C346" t="n">
-        <v>0</v>
+        <v>208</v>
       </c>
       <c r="D346" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E346" t="n">
-        <v>104</v>
+        <v>0</v>
       </c>
     </row>
     <row r="347">
@@ -6333,13 +6333,13 @@
         <v>16</v>
       </c>
       <c r="C347" t="n">
+        <v>0</v>
+      </c>
+      <c r="D347" t="n">
+        <v>0</v>
+      </c>
+      <c r="E347" t="n">
         <v>104</v>
-      </c>
-      <c r="D347" t="n">
-        <v>1</v>
-      </c>
-      <c r="E347" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="348">
@@ -6350,7 +6350,7 @@
         <v>17</v>
       </c>
       <c r="C348" t="n">
-        <v>104</v>
+        <v>208</v>
       </c>
       <c r="D348" t="n">
         <v>1</v>
@@ -6367,13 +6367,13 @@
         <v>18</v>
       </c>
       <c r="C349" t="n">
-        <v>208</v>
+        <v>0</v>
       </c>
       <c r="D349" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E349" t="n">
-        <v>0</v>
+        <v>104</v>
       </c>
     </row>
     <row r="350">
@@ -6384,13 +6384,13 @@
         <v>19</v>
       </c>
       <c r="C350" t="n">
-        <v>0</v>
+        <v>208</v>
       </c>
       <c r="D350" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E350" t="n">
-        <v>104</v>
+        <v>0</v>
       </c>
     </row>
     <row r="351">
@@ -6401,13 +6401,13 @@
         <v>20</v>
       </c>
       <c r="C351" t="n">
-        <v>208</v>
+        <v>0</v>
       </c>
       <c r="D351" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E351" t="n">
-        <v>0</v>
+        <v>104</v>
       </c>
     </row>
     <row r="352">
@@ -6418,13 +6418,13 @@
         <v>21</v>
       </c>
       <c r="C352" t="n">
-        <v>0</v>
+        <v>208</v>
       </c>
       <c r="D352" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E352" t="n">
-        <v>104</v>
+        <v>0</v>
       </c>
     </row>
     <row r="353">
@@ -6435,13 +6435,13 @@
         <v>22</v>
       </c>
       <c r="C353" t="n">
-        <v>208</v>
+        <v>0</v>
       </c>
       <c r="D353" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E353" t="n">
-        <v>0</v>
+        <v>104</v>
       </c>
     </row>
     <row r="354">
@@ -6452,13 +6452,13 @@
         <v>23</v>
       </c>
       <c r="C354" t="n">
-        <v>0</v>
+        <v>208</v>
       </c>
       <c r="D354" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E354" t="n">
-        <v>104</v>
+        <v>0</v>
       </c>
     </row>
     <row r="355">
@@ -6469,13 +6469,13 @@
         <v>24</v>
       </c>
       <c r="C355" t="n">
-        <v>208</v>
+        <v>0</v>
       </c>
       <c r="D355" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E355" t="n">
-        <v>0</v>
+        <v>104</v>
       </c>
     </row>
     <row r="356">
@@ -6486,13 +6486,13 @@
         <v>25</v>
       </c>
       <c r="C356" t="n">
-        <v>0</v>
+        <v>208</v>
       </c>
       <c r="D356" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E356" t="n">
-        <v>104</v>
+        <v>0</v>
       </c>
     </row>
     <row r="357">
@@ -6503,13 +6503,13 @@
         <v>26</v>
       </c>
       <c r="C357" t="n">
-        <v>208</v>
+        <v>0</v>
       </c>
       <c r="D357" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E357" t="n">
-        <v>0</v>
+        <v>104</v>
       </c>
     </row>
     <row r="358">
@@ -6520,13 +6520,13 @@
         <v>27</v>
       </c>
       <c r="C358" t="n">
-        <v>0</v>
+        <v>208</v>
       </c>
       <c r="D358" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E358" t="n">
-        <v>104</v>
+        <v>0</v>
       </c>
     </row>
     <row r="359">
@@ -6537,13 +6537,13 @@
         <v>28</v>
       </c>
       <c r="C359" t="n">
-        <v>208</v>
+        <v>0</v>
       </c>
       <c r="D359" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E359" t="n">
-        <v>0</v>
+        <v>104</v>
       </c>
     </row>
     <row r="360">
@@ -6554,13 +6554,13 @@
         <v>29</v>
       </c>
       <c r="C360" t="n">
-        <v>0</v>
+        <v>104</v>
       </c>
       <c r="D360" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E360" t="n">
-        <v>104</v>
+        <v>0</v>
       </c>
     </row>
     <row r="361">
@@ -6571,7 +6571,7 @@
         <v>30</v>
       </c>
       <c r="C361" t="n">
-        <v>4105</v>
+        <v>0</v>
       </c>
       <c r="D361" t="n">
         <v>1</v>
@@ -6591,10 +6591,10 @@
         <v>0</v>
       </c>
       <c r="D362" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E362" t="n">
-        <v>69</v>
+        <v>207</v>
       </c>
     </row>
     <row r="363">
@@ -6605,13 +6605,13 @@
         <v>2</v>
       </c>
       <c r="C363" t="n">
+        <v>0</v>
+      </c>
+      <c r="D363" t="n">
+        <v>0</v>
+      </c>
+      <c r="E363" t="n">
         <v>138</v>
-      </c>
-      <c r="D363" t="n">
-        <v>1</v>
-      </c>
-      <c r="E363" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="364">
@@ -6639,7 +6639,7 @@
         <v>4</v>
       </c>
       <c r="C365" t="n">
-        <v>138</v>
+        <v>207</v>
       </c>
       <c r="D365" t="n">
         <v>1</v>
@@ -6662,7 +6662,7 @@
         <v>0</v>
       </c>
       <c r="E366" t="n">
-        <v>69</v>
+        <v>138</v>
       </c>
     </row>
     <row r="367">
@@ -6673,13 +6673,13 @@
         <v>6</v>
       </c>
       <c r="C367" t="n">
-        <v>138</v>
+        <v>0</v>
       </c>
       <c r="D367" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E367" t="n">
-        <v>0</v>
+        <v>69</v>
       </c>
     </row>
     <row r="368">
@@ -6690,13 +6690,13 @@
         <v>7</v>
       </c>
       <c r="C368" t="n">
-        <v>0</v>
+        <v>207</v>
       </c>
       <c r="D368" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E368" t="n">
-        <v>69</v>
+        <v>0</v>
       </c>
     </row>
     <row r="369">
@@ -6707,13 +6707,13 @@
         <v>8</v>
       </c>
       <c r="C369" t="n">
+        <v>0</v>
+      </c>
+      <c r="D369" t="n">
+        <v>0</v>
+      </c>
+      <c r="E369" t="n">
         <v>138</v>
-      </c>
-      <c r="D369" t="n">
-        <v>1</v>
-      </c>
-      <c r="E369" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="370">
@@ -6741,7 +6741,7 @@
         <v>10</v>
       </c>
       <c r="C371" t="n">
-        <v>138</v>
+        <v>207</v>
       </c>
       <c r="D371" t="n">
         <v>1</v>
@@ -6764,7 +6764,7 @@
         <v>0</v>
       </c>
       <c r="E372" t="n">
-        <v>69</v>
+        <v>138</v>
       </c>
     </row>
     <row r="373">
@@ -6775,13 +6775,13 @@
         <v>12</v>
       </c>
       <c r="C373" t="n">
-        <v>138</v>
+        <v>0</v>
       </c>
       <c r="D373" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E373" t="n">
-        <v>0</v>
+        <v>69</v>
       </c>
     </row>
     <row r="374">
@@ -6792,13 +6792,13 @@
         <v>13</v>
       </c>
       <c r="C374" t="n">
-        <v>0</v>
+        <v>207</v>
       </c>
       <c r="D374" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E374" t="n">
-        <v>69</v>
+        <v>0</v>
       </c>
     </row>
     <row r="375">
@@ -6809,13 +6809,13 @@
         <v>14</v>
       </c>
       <c r="C375" t="n">
+        <v>0</v>
+      </c>
+      <c r="D375" t="n">
+        <v>0</v>
+      </c>
+      <c r="E375" t="n">
         <v>138</v>
-      </c>
-      <c r="D375" t="n">
-        <v>1</v>
-      </c>
-      <c r="E375" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="376">
@@ -6843,7 +6843,7 @@
         <v>16</v>
       </c>
       <c r="C377" t="n">
-        <v>138</v>
+        <v>207</v>
       </c>
       <c r="D377" t="n">
         <v>1</v>
@@ -6866,7 +6866,7 @@
         <v>0</v>
       </c>
       <c r="E378" t="n">
-        <v>69</v>
+        <v>138</v>
       </c>
     </row>
     <row r="379">
@@ -6877,13 +6877,13 @@
         <v>18</v>
       </c>
       <c r="C379" t="n">
-        <v>138</v>
+        <v>0</v>
       </c>
       <c r="D379" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E379" t="n">
-        <v>0</v>
+        <v>69</v>
       </c>
     </row>
     <row r="380">
@@ -6894,13 +6894,13 @@
         <v>19</v>
       </c>
       <c r="C380" t="n">
-        <v>0</v>
+        <v>207</v>
       </c>
       <c r="D380" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E380" t="n">
-        <v>69</v>
+        <v>0</v>
       </c>
     </row>
     <row r="381">
@@ -6911,13 +6911,13 @@
         <v>20</v>
       </c>
       <c r="C381" t="n">
-        <v>237</v>
+        <v>0</v>
       </c>
       <c r="D381" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E381" t="n">
-        <v>0</v>
+        <v>138</v>
       </c>
     </row>
     <row r="382">
@@ -6934,7 +6934,7 @@
         <v>0</v>
       </c>
       <c r="E382" t="n">
-        <v>168</v>
+        <v>69</v>
       </c>
     </row>
     <row r="383">
@@ -6945,13 +6945,13 @@
         <v>22</v>
       </c>
       <c r="C383" t="n">
-        <v>0</v>
+        <v>207</v>
       </c>
       <c r="D383" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E383" t="n">
-        <v>99</v>
+        <v>0</v>
       </c>
     </row>
     <row r="384">
@@ -6962,13 +6962,13 @@
         <v>23</v>
       </c>
       <c r="C384" t="n">
-        <v>108</v>
+        <v>0</v>
       </c>
       <c r="D384" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E384" t="n">
-        <v>30</v>
+        <v>138</v>
       </c>
     </row>
     <row r="385">
@@ -6996,7 +6996,7 @@
         <v>25</v>
       </c>
       <c r="C386" t="n">
-        <v>345</v>
+        <v>207</v>
       </c>
       <c r="D386" t="n">
         <v>1</v>
@@ -7019,7 +7019,7 @@
         <v>0</v>
       </c>
       <c r="E387" t="n">
-        <v>276</v>
+        <v>138</v>
       </c>
     </row>
     <row r="388">
@@ -7036,7 +7036,7 @@
         <v>0</v>
       </c>
       <c r="E388" t="n">
-        <v>207</v>
+        <v>69</v>
       </c>
     </row>
     <row r="389">
@@ -7047,13 +7047,13 @@
         <v>28</v>
       </c>
       <c r="C389" t="n">
-        <v>0</v>
+        <v>138</v>
       </c>
       <c r="D389" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E389" t="n">
-        <v>138</v>
+        <v>0</v>
       </c>
     </row>
     <row r="390">
@@ -7098,13 +7098,13 @@
         <v>1</v>
       </c>
       <c r="C392" t="n">
+        <v>0</v>
+      </c>
+      <c r="D392" t="n">
+        <v>1</v>
+      </c>
+      <c r="E392" t="n">
         <v>114</v>
-      </c>
-      <c r="D392" t="n">
-        <v>1</v>
-      </c>
-      <c r="E392" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="393">
@@ -7115,7 +7115,7 @@
         <v>2</v>
       </c>
       <c r="C393" t="n">
-        <v>114</v>
+        <v>228</v>
       </c>
       <c r="D393" t="n">
         <v>1</v>
@@ -7132,13 +7132,13 @@
         <v>3</v>
       </c>
       <c r="C394" t="n">
+        <v>0</v>
+      </c>
+      <c r="D394" t="n">
+        <v>0</v>
+      </c>
+      <c r="E394" t="n">
         <v>114</v>
-      </c>
-      <c r="D394" t="n">
-        <v>1</v>
-      </c>
-      <c r="E394" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="395">
@@ -7149,7 +7149,7 @@
         <v>4</v>
       </c>
       <c r="C395" t="n">
-        <v>114</v>
+        <v>228</v>
       </c>
       <c r="D395" t="n">
         <v>1</v>
@@ -7166,13 +7166,13 @@
         <v>5</v>
       </c>
       <c r="C396" t="n">
+        <v>0</v>
+      </c>
+      <c r="D396" t="n">
+        <v>0</v>
+      </c>
+      <c r="E396" t="n">
         <v>114</v>
-      </c>
-      <c r="D396" t="n">
-        <v>1</v>
-      </c>
-      <c r="E396" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="397">
@@ -7183,7 +7183,7 @@
         <v>6</v>
       </c>
       <c r="C397" t="n">
-        <v>114</v>
+        <v>228</v>
       </c>
       <c r="D397" t="n">
         <v>1</v>
@@ -7200,13 +7200,13 @@
         <v>7</v>
       </c>
       <c r="C398" t="n">
+        <v>0</v>
+      </c>
+      <c r="D398" t="n">
+        <v>0</v>
+      </c>
+      <c r="E398" t="n">
         <v>114</v>
-      </c>
-      <c r="D398" t="n">
-        <v>1</v>
-      </c>
-      <c r="E398" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="399">
@@ -7217,7 +7217,7 @@
         <v>8</v>
       </c>
       <c r="C399" t="n">
-        <v>114</v>
+        <v>228</v>
       </c>
       <c r="D399" t="n">
         <v>1</v>
@@ -7234,13 +7234,13 @@
         <v>9</v>
       </c>
       <c r="C400" t="n">
+        <v>0</v>
+      </c>
+      <c r="D400" t="n">
+        <v>0</v>
+      </c>
+      <c r="E400" t="n">
         <v>114</v>
-      </c>
-      <c r="D400" t="n">
-        <v>1</v>
-      </c>
-      <c r="E400" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="401">
@@ -7251,7 +7251,7 @@
         <v>10</v>
       </c>
       <c r="C401" t="n">
-        <v>114</v>
+        <v>228</v>
       </c>
       <c r="D401" t="n">
         <v>1</v>
@@ -7268,13 +7268,13 @@
         <v>11</v>
       </c>
       <c r="C402" t="n">
+        <v>0</v>
+      </c>
+      <c r="D402" t="n">
+        <v>0</v>
+      </c>
+      <c r="E402" t="n">
         <v>114</v>
-      </c>
-      <c r="D402" t="n">
-        <v>1</v>
-      </c>
-      <c r="E402" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="403">
@@ -7285,7 +7285,7 @@
         <v>12</v>
       </c>
       <c r="C403" t="n">
-        <v>114</v>
+        <v>228</v>
       </c>
       <c r="D403" t="n">
         <v>1</v>
@@ -7302,13 +7302,13 @@
         <v>13</v>
       </c>
       <c r="C404" t="n">
+        <v>0</v>
+      </c>
+      <c r="D404" t="n">
+        <v>0</v>
+      </c>
+      <c r="E404" t="n">
         <v>114</v>
-      </c>
-      <c r="D404" t="n">
-        <v>1</v>
-      </c>
-      <c r="E404" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="405">
@@ -7319,7 +7319,7 @@
         <v>14</v>
       </c>
       <c r="C405" t="n">
-        <v>114</v>
+        <v>228</v>
       </c>
       <c r="D405" t="n">
         <v>1</v>
@@ -7336,13 +7336,13 @@
         <v>15</v>
       </c>
       <c r="C406" t="n">
+        <v>0</v>
+      </c>
+      <c r="D406" t="n">
+        <v>0</v>
+      </c>
+      <c r="E406" t="n">
         <v>114</v>
-      </c>
-      <c r="D406" t="n">
-        <v>1</v>
-      </c>
-      <c r="E406" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="407">
@@ -7353,7 +7353,7 @@
         <v>16</v>
       </c>
       <c r="C407" t="n">
-        <v>114</v>
+        <v>228</v>
       </c>
       <c r="D407" t="n">
         <v>1</v>
@@ -7370,13 +7370,13 @@
         <v>17</v>
       </c>
       <c r="C408" t="n">
+        <v>0</v>
+      </c>
+      <c r="D408" t="n">
+        <v>0</v>
+      </c>
+      <c r="E408" t="n">
         <v>114</v>
-      </c>
-      <c r="D408" t="n">
-        <v>1</v>
-      </c>
-      <c r="E408" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="409">
@@ -7455,7 +7455,7 @@
         <v>22</v>
       </c>
       <c r="C413" t="n">
-        <v>333</v>
+        <v>228</v>
       </c>
       <c r="D413" t="n">
         <v>1</v>
@@ -7478,7 +7478,7 @@
         <v>0</v>
       </c>
       <c r="E414" t="n">
-        <v>219</v>
+        <v>114</v>
       </c>
     </row>
     <row r="415">
@@ -7489,13 +7489,13 @@
         <v>24</v>
       </c>
       <c r="C415" t="n">
-        <v>176</v>
+        <v>228</v>
       </c>
       <c r="D415" t="n">
         <v>1</v>
       </c>
       <c r="E415" t="n">
-        <v>105</v>
+        <v>0</v>
       </c>
     </row>
     <row r="416">
@@ -7512,7 +7512,7 @@
         <v>0</v>
       </c>
       <c r="E416" t="n">
-        <v>167</v>
+        <v>114</v>
       </c>
     </row>
     <row r="417">
@@ -7523,13 +7523,13 @@
         <v>26</v>
       </c>
       <c r="C417" t="n">
-        <v>61</v>
+        <v>228</v>
       </c>
       <c r="D417" t="n">
         <v>1</v>
       </c>
       <c r="E417" t="n">
-        <v>53</v>
+        <v>0</v>
       </c>
     </row>
     <row r="418">
@@ -7540,13 +7540,13 @@
         <v>27</v>
       </c>
       <c r="C418" t="n">
-        <v>342</v>
+        <v>0</v>
       </c>
       <c r="D418" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E418" t="n">
-        <v>0</v>
+        <v>114</v>
       </c>
     </row>
     <row r="419">
@@ -7557,13 +7557,13 @@
         <v>28</v>
       </c>
       <c r="C419" t="n">
-        <v>0</v>
+        <v>228</v>
       </c>
       <c r="D419" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E419" t="n">
-        <v>228</v>
+        <v>0</v>
       </c>
     </row>
     <row r="420">
@@ -7594,7 +7594,7 @@
         <v>0</v>
       </c>
       <c r="D421" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E421" t="n">
         <v>0</v>
@@ -7608,13 +7608,13 @@
         <v>1</v>
       </c>
       <c r="C422" t="n">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D422" t="n">
         <v>1</v>
       </c>
       <c r="E422" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
     </row>
     <row r="423">
@@ -7625,13 +7625,13 @@
         <v>2</v>
       </c>
       <c r="C423" t="n">
+        <v>0</v>
+      </c>
+      <c r="D423" t="n">
+        <v>0</v>
+      </c>
+      <c r="E423" t="n">
         <v>150</v>
-      </c>
-      <c r="D423" t="n">
-        <v>1</v>
-      </c>
-      <c r="E423" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="424">
@@ -7642,7 +7642,7 @@
         <v>3</v>
       </c>
       <c r="C424" t="n">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="D424" t="n">
         <v>1</v>
@@ -7659,13 +7659,13 @@
         <v>4</v>
       </c>
       <c r="C425" t="n">
+        <v>0</v>
+      </c>
+      <c r="D425" t="n">
+        <v>0</v>
+      </c>
+      <c r="E425" t="n">
         <v>150</v>
-      </c>
-      <c r="D425" t="n">
-        <v>1</v>
-      </c>
-      <c r="E425" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="426">
@@ -7676,7 +7676,7 @@
         <v>5</v>
       </c>
       <c r="C426" t="n">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="D426" t="n">
         <v>1</v>
@@ -7693,13 +7693,13 @@
         <v>6</v>
       </c>
       <c r="C427" t="n">
+        <v>0</v>
+      </c>
+      <c r="D427" t="n">
+        <v>0</v>
+      </c>
+      <c r="E427" t="n">
         <v>150</v>
-      </c>
-      <c r="D427" t="n">
-        <v>1</v>
-      </c>
-      <c r="E427" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="428">
@@ -7710,7 +7710,7 @@
         <v>7</v>
       </c>
       <c r="C428" t="n">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="D428" t="n">
         <v>1</v>
@@ -7727,13 +7727,13 @@
         <v>8</v>
       </c>
       <c r="C429" t="n">
+        <v>0</v>
+      </c>
+      <c r="D429" t="n">
+        <v>0</v>
+      </c>
+      <c r="E429" t="n">
         <v>150</v>
-      </c>
-      <c r="D429" t="n">
-        <v>1</v>
-      </c>
-      <c r="E429" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="430">
@@ -7744,7 +7744,7 @@
         <v>9</v>
       </c>
       <c r="C430" t="n">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="D430" t="n">
         <v>1</v>
@@ -7761,13 +7761,13 @@
         <v>10</v>
       </c>
       <c r="C431" t="n">
+        <v>0</v>
+      </c>
+      <c r="D431" t="n">
+        <v>0</v>
+      </c>
+      <c r="E431" t="n">
         <v>150</v>
-      </c>
-      <c r="D431" t="n">
-        <v>1</v>
-      </c>
-      <c r="E431" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="432">
@@ -7778,7 +7778,7 @@
         <v>11</v>
       </c>
       <c r="C432" t="n">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="D432" t="n">
         <v>1</v>
@@ -7795,13 +7795,13 @@
         <v>12</v>
       </c>
       <c r="C433" t="n">
+        <v>0</v>
+      </c>
+      <c r="D433" t="n">
+        <v>0</v>
+      </c>
+      <c r="E433" t="n">
         <v>150</v>
-      </c>
-      <c r="D433" t="n">
-        <v>1</v>
-      </c>
-      <c r="E433" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="434">
@@ -7812,7 +7812,7 @@
         <v>13</v>
       </c>
       <c r="C434" t="n">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="D434" t="n">
         <v>1</v>
@@ -7829,13 +7829,13 @@
         <v>14</v>
       </c>
       <c r="C435" t="n">
+        <v>0</v>
+      </c>
+      <c r="D435" t="n">
+        <v>0</v>
+      </c>
+      <c r="E435" t="n">
         <v>150</v>
-      </c>
-      <c r="D435" t="n">
-        <v>1</v>
-      </c>
-      <c r="E435" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="436">
@@ -7846,7 +7846,7 @@
         <v>15</v>
       </c>
       <c r="C436" t="n">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="D436" t="n">
         <v>1</v>
@@ -7863,13 +7863,13 @@
         <v>16</v>
       </c>
       <c r="C437" t="n">
+        <v>0</v>
+      </c>
+      <c r="D437" t="n">
+        <v>0</v>
+      </c>
+      <c r="E437" t="n">
         <v>150</v>
-      </c>
-      <c r="D437" t="n">
-        <v>1</v>
-      </c>
-      <c r="E437" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="438">
@@ -7880,7 +7880,7 @@
         <v>17</v>
       </c>
       <c r="C438" t="n">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="D438" t="n">
         <v>1</v>
@@ -7897,13 +7897,13 @@
         <v>18</v>
       </c>
       <c r="C439" t="n">
+        <v>0</v>
+      </c>
+      <c r="D439" t="n">
+        <v>0</v>
+      </c>
+      <c r="E439" t="n">
         <v>150</v>
-      </c>
-      <c r="D439" t="n">
-        <v>1</v>
-      </c>
-      <c r="E439" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="440">
@@ -7982,7 +7982,7 @@
         <v>23</v>
       </c>
       <c r="C444" t="n">
-        <v>387</v>
+        <v>300</v>
       </c>
       <c r="D444" t="n">
         <v>1</v>
@@ -8005,7 +8005,7 @@
         <v>0</v>
       </c>
       <c r="E445" t="n">
-        <v>237</v>
+        <v>150</v>
       </c>
     </row>
     <row r="446">
@@ -8016,13 +8016,13 @@
         <v>25</v>
       </c>
       <c r="C446" t="n">
-        <v>213</v>
+        <v>300</v>
       </c>
       <c r="D446" t="n">
         <v>1</v>
       </c>
       <c r="E446" t="n">
-        <v>87</v>
+        <v>0</v>
       </c>
     </row>
     <row r="447">
@@ -8036,7 +8036,7 @@
         <v>0</v>
       </c>
       <c r="D447" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E447" t="n">
         <v>150</v>
@@ -8050,7 +8050,7 @@
         <v>27</v>
       </c>
       <c r="C448" t="n">
-        <v>330</v>
+        <v>300</v>
       </c>
       <c r="D448" t="n">
         <v>1</v>
@@ -8067,13 +8067,13 @@
         <v>28</v>
       </c>
       <c r="C449" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="D449" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E449" t="n">
-        <v>180</v>
+        <v>150</v>
       </c>
     </row>
     <row r="450">
@@ -8084,13 +8084,13 @@
         <v>29</v>
       </c>
       <c r="C450" t="n">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="D450" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E450" t="n">
-        <v>150</v>
+        <v>0</v>
       </c>
     </row>
     <row r="451">
@@ -8152,7 +8152,7 @@
         <v>3</v>
       </c>
       <c r="C454" t="n">
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="D454" t="n">
         <v>1</v>
@@ -8169,13 +8169,13 @@
         <v>4</v>
       </c>
       <c r="C455" t="n">
+        <v>0</v>
+      </c>
+      <c r="D455" t="n">
+        <v>0</v>
+      </c>
+      <c r="E455" t="n">
         <v>160</v>
-      </c>
-      <c r="D455" t="n">
-        <v>1</v>
-      </c>
-      <c r="E455" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="456">
@@ -8186,7 +8186,7 @@
         <v>5</v>
       </c>
       <c r="C456" t="n">
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="D456" t="n">
         <v>1</v>
@@ -8203,13 +8203,13 @@
         <v>6</v>
       </c>
       <c r="C457" t="n">
+        <v>0</v>
+      </c>
+      <c r="D457" t="n">
+        <v>0</v>
+      </c>
+      <c r="E457" t="n">
         <v>160</v>
-      </c>
-      <c r="D457" t="n">
-        <v>1</v>
-      </c>
-      <c r="E457" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="458">
@@ -8220,7 +8220,7 @@
         <v>7</v>
       </c>
       <c r="C458" t="n">
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="D458" t="n">
         <v>1</v>
@@ -8237,13 +8237,13 @@
         <v>8</v>
       </c>
       <c r="C459" t="n">
+        <v>0</v>
+      </c>
+      <c r="D459" t="n">
+        <v>0</v>
+      </c>
+      <c r="E459" t="n">
         <v>160</v>
-      </c>
-      <c r="D459" t="n">
-        <v>1</v>
-      </c>
-      <c r="E459" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="460">
@@ -8254,7 +8254,7 @@
         <v>9</v>
       </c>
       <c r="C460" t="n">
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="D460" t="n">
         <v>1</v>
@@ -8271,13 +8271,13 @@
         <v>10</v>
       </c>
       <c r="C461" t="n">
+        <v>0</v>
+      </c>
+      <c r="D461" t="n">
+        <v>0</v>
+      </c>
+      <c r="E461" t="n">
         <v>160</v>
-      </c>
-      <c r="D461" t="n">
-        <v>1</v>
-      </c>
-      <c r="E461" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="462">
@@ -8288,7 +8288,7 @@
         <v>11</v>
       </c>
       <c r="C462" t="n">
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="D462" t="n">
         <v>1</v>
@@ -8305,13 +8305,13 @@
         <v>12</v>
       </c>
       <c r="C463" t="n">
+        <v>0</v>
+      </c>
+      <c r="D463" t="n">
+        <v>0</v>
+      </c>
+      <c r="E463" t="n">
         <v>160</v>
-      </c>
-      <c r="D463" t="n">
-        <v>1</v>
-      </c>
-      <c r="E463" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="464">
@@ -8322,7 +8322,7 @@
         <v>13</v>
       </c>
       <c r="C464" t="n">
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="D464" t="n">
         <v>1</v>
@@ -8339,13 +8339,13 @@
         <v>14</v>
       </c>
       <c r="C465" t="n">
+        <v>0</v>
+      </c>
+      <c r="D465" t="n">
+        <v>0</v>
+      </c>
+      <c r="E465" t="n">
         <v>160</v>
-      </c>
-      <c r="D465" t="n">
-        <v>1</v>
-      </c>
-      <c r="E465" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="466">
@@ -8356,7 +8356,7 @@
         <v>15</v>
       </c>
       <c r="C466" t="n">
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="D466" t="n">
         <v>1</v>
@@ -8373,13 +8373,13 @@
         <v>16</v>
       </c>
       <c r="C467" t="n">
+        <v>0</v>
+      </c>
+      <c r="D467" t="n">
+        <v>0</v>
+      </c>
+      <c r="E467" t="n">
         <v>160</v>
-      </c>
-      <c r="D467" t="n">
-        <v>1</v>
-      </c>
-      <c r="E467" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="468">
@@ -8390,7 +8390,7 @@
         <v>17</v>
       </c>
       <c r="C468" t="n">
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="D468" t="n">
         <v>1</v>
@@ -8407,13 +8407,13 @@
         <v>18</v>
       </c>
       <c r="C469" t="n">
+        <v>0</v>
+      </c>
+      <c r="D469" t="n">
+        <v>0</v>
+      </c>
+      <c r="E469" t="n">
         <v>160</v>
-      </c>
-      <c r="D469" t="n">
-        <v>1</v>
-      </c>
-      <c r="E469" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="470">
@@ -8424,7 +8424,7 @@
         <v>19</v>
       </c>
       <c r="C470" t="n">
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="D470" t="n">
         <v>1</v>
@@ -8441,13 +8441,13 @@
         <v>20</v>
       </c>
       <c r="C471" t="n">
-        <v>320</v>
+        <v>0</v>
       </c>
       <c r="D471" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E471" t="n">
-        <v>0</v>
+        <v>160</v>
       </c>
     </row>
     <row r="472">
@@ -8458,13 +8458,13 @@
         <v>21</v>
       </c>
       <c r="C472" t="n">
-        <v>0</v>
+        <v>320</v>
       </c>
       <c r="D472" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E472" t="n">
-        <v>160</v>
+        <v>0</v>
       </c>
     </row>
     <row r="473">
@@ -8475,13 +8475,13 @@
         <v>22</v>
       </c>
       <c r="C473" t="n">
-        <v>320</v>
+        <v>0</v>
       </c>
       <c r="D473" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E473" t="n">
-        <v>0</v>
+        <v>160</v>
       </c>
     </row>
     <row r="474">
@@ -8492,13 +8492,13 @@
         <v>23</v>
       </c>
       <c r="C474" t="n">
-        <v>0</v>
+        <v>320</v>
       </c>
       <c r="D474" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E474" t="n">
-        <v>160</v>
+        <v>0</v>
       </c>
     </row>
     <row r="475">
@@ -8509,13 +8509,13 @@
         <v>24</v>
       </c>
       <c r="C475" t="n">
-        <v>320</v>
+        <v>0</v>
       </c>
       <c r="D475" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E475" t="n">
-        <v>0</v>
+        <v>160</v>
       </c>
     </row>
     <row r="476">
@@ -8526,13 +8526,13 @@
         <v>25</v>
       </c>
       <c r="C476" t="n">
-        <v>0</v>
+        <v>320</v>
       </c>
       <c r="D476" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E476" t="n">
-        <v>160</v>
+        <v>0</v>
       </c>
     </row>
     <row r="477">
@@ -8543,13 +8543,13 @@
         <v>26</v>
       </c>
       <c r="C477" t="n">
+        <v>0</v>
+      </c>
+      <c r="D477" t="n">
+        <v>0</v>
+      </c>
+      <c r="E477" t="n">
         <v>160</v>
-      </c>
-      <c r="D477" t="n">
-        <v>1</v>
-      </c>
-      <c r="E477" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="478">
@@ -8580,7 +8580,7 @@
         <v>0</v>
       </c>
       <c r="D479" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E479" t="n">
         <v>160</v>
@@ -8614,7 +8614,7 @@
         <v>0</v>
       </c>
       <c r="D481" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E481" t="n">
         <v>0</v>
@@ -8628,13 +8628,13 @@
         <v>1</v>
       </c>
       <c r="C482" t="n">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="D482" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E482" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="483">
@@ -8645,13 +8645,13 @@
         <v>2</v>
       </c>
       <c r="C483" t="n">
+        <v>0</v>
+      </c>
+      <c r="D483" t="n">
+        <v>0</v>
+      </c>
+      <c r="E483" t="n">
         <v>54</v>
-      </c>
-      <c r="D483" t="n">
-        <v>1</v>
-      </c>
-      <c r="E483" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="484">
@@ -8696,7 +8696,7 @@
         <v>5</v>
       </c>
       <c r="C486" t="n">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="D486" t="n">
         <v>1</v>
@@ -8719,7 +8719,7 @@
         <v>0</v>
       </c>
       <c r="E487" t="n">
-        <v>36</v>
+        <v>90</v>
       </c>
     </row>
     <row r="488">
@@ -8736,7 +8736,7 @@
         <v>0</v>
       </c>
       <c r="E488" t="n">
-        <v>18</v>
+        <v>72</v>
       </c>
     </row>
     <row r="489">
@@ -8747,13 +8747,13 @@
         <v>8</v>
       </c>
       <c r="C489" t="n">
+        <v>0</v>
+      </c>
+      <c r="D489" t="n">
+        <v>0</v>
+      </c>
+      <c r="E489" t="n">
         <v>54</v>
-      </c>
-      <c r="D489" t="n">
-        <v>1</v>
-      </c>
-      <c r="E489" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="490">
@@ -8798,7 +8798,7 @@
         <v>11</v>
       </c>
       <c r="C492" t="n">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="D492" t="n">
         <v>1</v>
@@ -8821,7 +8821,7 @@
         <v>0</v>
       </c>
       <c r="E493" t="n">
-        <v>36</v>
+        <v>90</v>
       </c>
     </row>
     <row r="494">
@@ -8838,7 +8838,7 @@
         <v>0</v>
       </c>
       <c r="E494" t="n">
-        <v>18</v>
+        <v>72</v>
       </c>
     </row>
     <row r="495">
@@ -8849,13 +8849,13 @@
         <v>14</v>
       </c>
       <c r="C495" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="D495" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E495" t="n">
-        <v>0</v>
+        <v>54</v>
       </c>
     </row>
     <row r="496">
@@ -8872,7 +8872,7 @@
         <v>0</v>
       </c>
       <c r="E496" t="n">
-        <v>54</v>
+        <v>36</v>
       </c>
     </row>
     <row r="497">
@@ -8889,7 +8889,7 @@
         <v>0</v>
       </c>
       <c r="E497" t="n">
-        <v>36</v>
+        <v>18</v>
       </c>
     </row>
     <row r="498">
@@ -8900,13 +8900,13 @@
         <v>17</v>
       </c>
       <c r="C498" t="n">
-        <v>0</v>
+        <v>108</v>
       </c>
       <c r="D498" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E498" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="499">
@@ -8917,13 +8917,13 @@
         <v>18</v>
       </c>
       <c r="C499" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="D499" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E499" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="500">
@@ -8940,7 +8940,7 @@
         <v>0</v>
       </c>
       <c r="E500" t="n">
-        <v>54</v>
+        <v>72</v>
       </c>
     </row>
     <row r="501">
@@ -8957,7 +8957,7 @@
         <v>0</v>
       </c>
       <c r="E501" t="n">
-        <v>36</v>
+        <v>54</v>
       </c>
     </row>
     <row r="502">
@@ -8974,7 +8974,7 @@
         <v>0</v>
       </c>
       <c r="E502" t="n">
-        <v>18</v>
+        <v>36</v>
       </c>
     </row>
     <row r="503">
@@ -8985,13 +8985,13 @@
         <v>22</v>
       </c>
       <c r="C503" t="n">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="D503" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E503" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="504">
@@ -9002,13 +9002,13 @@
         <v>23</v>
       </c>
       <c r="C504" t="n">
-        <v>0</v>
+        <v>126</v>
       </c>
       <c r="D504" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E504" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="505">
@@ -9019,13 +9019,13 @@
         <v>24</v>
       </c>
       <c r="C505" t="n">
+        <v>0</v>
+      </c>
+      <c r="D505" t="n">
+        <v>0</v>
+      </c>
+      <c r="E505" t="n">
         <v>108</v>
-      </c>
-      <c r="D505" t="n">
-        <v>1</v>
-      </c>
-      <c r="E505" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="506">
@@ -9138,13 +9138,13 @@
         <v>1</v>
       </c>
       <c r="C512" t="n">
-        <v>0</v>
+        <v>126</v>
       </c>
       <c r="D512" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E512" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="513">
@@ -9155,13 +9155,13 @@
         <v>2</v>
       </c>
       <c r="C513" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="D513" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E513" t="n">
-        <v>0</v>
+        <v>108</v>
       </c>
     </row>
     <row r="514">
@@ -9178,7 +9178,7 @@
         <v>0</v>
       </c>
       <c r="E514" t="n">
-        <v>54</v>
+        <v>90</v>
       </c>
     </row>
     <row r="515">
@@ -9195,7 +9195,7 @@
         <v>0</v>
       </c>
       <c r="E515" t="n">
-        <v>36</v>
+        <v>72</v>
       </c>
     </row>
     <row r="516">
@@ -9212,7 +9212,7 @@
         <v>0</v>
       </c>
       <c r="E516" t="n">
-        <v>18</v>
+        <v>54</v>
       </c>
     </row>
     <row r="517">
@@ -9223,13 +9223,13 @@
         <v>6</v>
       </c>
       <c r="C517" t="n">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="D517" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E517" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
     </row>
     <row r="518">
@@ -9246,7 +9246,7 @@
         <v>0</v>
       </c>
       <c r="E518" t="n">
-        <v>36</v>
+        <v>18</v>
       </c>
     </row>
     <row r="519">
@@ -9257,13 +9257,13 @@
         <v>8</v>
       </c>
       <c r="C519" t="n">
-        <v>0</v>
+        <v>108</v>
       </c>
       <c r="D519" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E519" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="520">
@@ -9274,13 +9274,13 @@
         <v>9</v>
       </c>
       <c r="C520" t="n">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="D520" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E520" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="521">
@@ -9297,7 +9297,7 @@
         <v>0</v>
       </c>
       <c r="E521" t="n">
-        <v>36</v>
+        <v>72</v>
       </c>
     </row>
     <row r="522">
@@ -9314,7 +9314,7 @@
         <v>0</v>
       </c>
       <c r="E522" t="n">
-        <v>18</v>
+        <v>54</v>
       </c>
     </row>
     <row r="523">
@@ -9325,13 +9325,13 @@
         <v>12</v>
       </c>
       <c r="C523" t="n">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="D523" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E523" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
     </row>
     <row r="524">
@@ -9348,7 +9348,7 @@
         <v>0</v>
       </c>
       <c r="E524" t="n">
-        <v>36</v>
+        <v>18</v>
       </c>
     </row>
     <row r="525">
@@ -9359,13 +9359,13 @@
         <v>14</v>
       </c>
       <c r="C525" t="n">
-        <v>0</v>
+        <v>108</v>
       </c>
       <c r="D525" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E525" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="526">
@@ -9376,13 +9376,13 @@
         <v>15</v>
       </c>
       <c r="C526" t="n">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="D526" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E526" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="527">
@@ -9399,7 +9399,7 @@
         <v>0</v>
       </c>
       <c r="E527" t="n">
-        <v>36</v>
+        <v>72</v>
       </c>
     </row>
     <row r="528">
@@ -9416,7 +9416,7 @@
         <v>0</v>
       </c>
       <c r="E528" t="n">
-        <v>18</v>
+        <v>54</v>
       </c>
     </row>
     <row r="529">
@@ -9427,13 +9427,13 @@
         <v>18</v>
       </c>
       <c r="C529" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="D529" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E529" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
     </row>
     <row r="530">
@@ -9450,7 +9450,7 @@
         <v>0</v>
       </c>
       <c r="E530" t="n">
-        <v>54</v>
+        <v>18</v>
       </c>
     </row>
     <row r="531">
@@ -9461,13 +9461,13 @@
         <v>20</v>
       </c>
       <c r="C531" t="n">
-        <v>0</v>
+        <v>108</v>
       </c>
       <c r="D531" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E531" t="n">
-        <v>36</v>
+        <v>0</v>
       </c>
     </row>
     <row r="532">
@@ -9484,7 +9484,7 @@
         <v>0</v>
       </c>
       <c r="E532" t="n">
-        <v>18</v>
+        <v>90</v>
       </c>
     </row>
     <row r="533">
@@ -9495,13 +9495,13 @@
         <v>22</v>
       </c>
       <c r="C533" t="n">
+        <v>0</v>
+      </c>
+      <c r="D533" t="n">
+        <v>0</v>
+      </c>
+      <c r="E533" t="n">
         <v>72</v>
-      </c>
-      <c r="D533" t="n">
-        <v>1</v>
-      </c>
-      <c r="E533" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="534">
@@ -9563,7 +9563,7 @@
         <v>26</v>
       </c>
       <c r="C537" t="n">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="D537" t="n">
         <v>1</v>
@@ -9586,7 +9586,7 @@
         <v>0</v>
       </c>
       <c r="E538" t="n">
-        <v>36</v>
+        <v>54</v>
       </c>
     </row>
     <row r="539">
@@ -9603,7 +9603,7 @@
         <v>0</v>
       </c>
       <c r="E539" t="n">
-        <v>18</v>
+        <v>36</v>
       </c>
     </row>
     <row r="540">
@@ -9614,13 +9614,13 @@
         <v>29</v>
       </c>
       <c r="C540" t="n">
+        <v>0</v>
+      </c>
+      <c r="D540" t="n">
+        <v>0</v>
+      </c>
+      <c r="E540" t="n">
         <v>18</v>
-      </c>
-      <c r="D540" t="n">
-        <v>1</v>
-      </c>
-      <c r="E540" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="541">
@@ -9648,13 +9648,13 @@
         <v>1</v>
       </c>
       <c r="C542" t="n">
+        <v>0</v>
+      </c>
+      <c r="D542" t="n">
+        <v>0</v>
+      </c>
+      <c r="E542" t="n">
         <v>160</v>
-      </c>
-      <c r="D542" t="n">
-        <v>1</v>
-      </c>
-      <c r="E542" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="543">
@@ -9665,7 +9665,7 @@
         <v>2</v>
       </c>
       <c r="C543" t="n">
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="D543" t="n">
         <v>1</v>
@@ -9682,13 +9682,13 @@
         <v>3</v>
       </c>
       <c r="C544" t="n">
+        <v>0</v>
+      </c>
+      <c r="D544" t="n">
+        <v>0</v>
+      </c>
+      <c r="E544" t="n">
         <v>160</v>
-      </c>
-      <c r="D544" t="n">
-        <v>1</v>
-      </c>
-      <c r="E544" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="545">
@@ -9699,7 +9699,7 @@
         <v>4</v>
       </c>
       <c r="C545" t="n">
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="D545" t="n">
         <v>1</v>
@@ -9716,13 +9716,13 @@
         <v>5</v>
       </c>
       <c r="C546" t="n">
+        <v>0</v>
+      </c>
+      <c r="D546" t="n">
+        <v>0</v>
+      </c>
+      <c r="E546" t="n">
         <v>160</v>
-      </c>
-      <c r="D546" t="n">
-        <v>1</v>
-      </c>
-      <c r="E546" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="547">
@@ -9733,7 +9733,7 @@
         <v>6</v>
       </c>
       <c r="C547" t="n">
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="D547" t="n">
         <v>1</v>
@@ -9750,13 +9750,13 @@
         <v>7</v>
       </c>
       <c r="C548" t="n">
+        <v>0</v>
+      </c>
+      <c r="D548" t="n">
+        <v>0</v>
+      </c>
+      <c r="E548" t="n">
         <v>160</v>
-      </c>
-      <c r="D548" t="n">
-        <v>1</v>
-      </c>
-      <c r="E548" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="549">
@@ -9767,7 +9767,7 @@
         <v>8</v>
       </c>
       <c r="C549" t="n">
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="D549" t="n">
         <v>1</v>
@@ -9784,13 +9784,13 @@
         <v>9</v>
       </c>
       <c r="C550" t="n">
+        <v>0</v>
+      </c>
+      <c r="D550" t="n">
+        <v>0</v>
+      </c>
+      <c r="E550" t="n">
         <v>160</v>
-      </c>
-      <c r="D550" t="n">
-        <v>1</v>
-      </c>
-      <c r="E550" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="551">
@@ -9801,7 +9801,7 @@
         <v>10</v>
       </c>
       <c r="C551" t="n">
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="D551" t="n">
         <v>1</v>
@@ -9818,13 +9818,13 @@
         <v>11</v>
       </c>
       <c r="C552" t="n">
+        <v>0</v>
+      </c>
+      <c r="D552" t="n">
+        <v>0</v>
+      </c>
+      <c r="E552" t="n">
         <v>160</v>
-      </c>
-      <c r="D552" t="n">
-        <v>1</v>
-      </c>
-      <c r="E552" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="553">
@@ -9835,7 +9835,7 @@
         <v>12</v>
       </c>
       <c r="C553" t="n">
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="D553" t="n">
         <v>1</v>
@@ -9852,13 +9852,13 @@
         <v>13</v>
       </c>
       <c r="C554" t="n">
+        <v>0</v>
+      </c>
+      <c r="D554" t="n">
+        <v>0</v>
+      </c>
+      <c r="E554" t="n">
         <v>160</v>
-      </c>
-      <c r="D554" t="n">
-        <v>1</v>
-      </c>
-      <c r="E554" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="555">
@@ -9869,7 +9869,7 @@
         <v>14</v>
       </c>
       <c r="C555" t="n">
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="D555" t="n">
         <v>1</v>
@@ -9886,13 +9886,13 @@
         <v>15</v>
       </c>
       <c r="C556" t="n">
+        <v>0</v>
+      </c>
+      <c r="D556" t="n">
+        <v>0</v>
+      </c>
+      <c r="E556" t="n">
         <v>160</v>
-      </c>
-      <c r="D556" t="n">
-        <v>1</v>
-      </c>
-      <c r="E556" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="557">
@@ -9903,7 +9903,7 @@
         <v>16</v>
       </c>
       <c r="C557" t="n">
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="D557" t="n">
         <v>1</v>
@@ -9920,13 +9920,13 @@
         <v>17</v>
       </c>
       <c r="C558" t="n">
+        <v>0</v>
+      </c>
+      <c r="D558" t="n">
+        <v>0</v>
+      </c>
+      <c r="E558" t="n">
         <v>160</v>
-      </c>
-      <c r="D558" t="n">
-        <v>1</v>
-      </c>
-      <c r="E558" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="559">
@@ -9937,7 +9937,7 @@
         <v>18</v>
       </c>
       <c r="C559" t="n">
-        <v>254</v>
+        <v>320</v>
       </c>
       <c r="D559" t="n">
         <v>1</v>
@@ -9954,13 +9954,13 @@
         <v>19</v>
       </c>
       <c r="C560" t="n">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="D560" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E560" t="n">
-        <v>94</v>
+        <v>160</v>
       </c>
     </row>
     <row r="561">
@@ -9971,7 +9971,7 @@
         <v>20</v>
       </c>
       <c r="C561" t="n">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="D561" t="n">
         <v>1</v>
@@ -9994,7 +9994,7 @@
         <v>0</v>
       </c>
       <c r="E562" t="n">
-        <v>170</v>
+        <v>160</v>
       </c>
     </row>
     <row r="563">
@@ -10005,13 +10005,13 @@
         <v>22</v>
       </c>
       <c r="C563" t="n">
-        <v>310</v>
+        <v>320</v>
       </c>
       <c r="D563" t="n">
         <v>1</v>
       </c>
       <c r="E563" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="564">
@@ -10039,7 +10039,7 @@
         <v>24</v>
       </c>
       <c r="C565" t="n">
-        <v>480</v>
+        <v>320</v>
       </c>
       <c r="D565" t="n">
         <v>1</v>
@@ -10062,7 +10062,7 @@
         <v>0</v>
       </c>
       <c r="E566" t="n">
-        <v>320</v>
+        <v>160</v>
       </c>
     </row>
     <row r="567">
@@ -10073,13 +10073,13 @@
         <v>26</v>
       </c>
       <c r="C567" t="n">
-        <v>0</v>
+        <v>320</v>
       </c>
       <c r="D567" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E567" t="n">
-        <v>160</v>
+        <v>0</v>
       </c>
     </row>
     <row r="568">
@@ -10090,13 +10090,13 @@
         <v>27</v>
       </c>
       <c r="C568" t="n">
+        <v>0</v>
+      </c>
+      <c r="D568" t="n">
+        <v>0</v>
+      </c>
+      <c r="E568" t="n">
         <v>160</v>
-      </c>
-      <c r="D568" t="n">
-        <v>1</v>
-      </c>
-      <c r="E568" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="569">
@@ -10158,13 +10158,13 @@
         <v>1</v>
       </c>
       <c r="C572" t="n">
+        <v>0</v>
+      </c>
+      <c r="D572" t="n">
+        <v>1</v>
+      </c>
+      <c r="E572" t="n">
         <v>150</v>
-      </c>
-      <c r="D572" t="n">
-        <v>1</v>
-      </c>
-      <c r="E572" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="573">
@@ -10175,7 +10175,7 @@
         <v>2</v>
       </c>
       <c r="C573" t="n">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="D573" t="n">
         <v>1</v>
@@ -10192,13 +10192,13 @@
         <v>3</v>
       </c>
       <c r="C574" t="n">
+        <v>0</v>
+      </c>
+      <c r="D574" t="n">
+        <v>0</v>
+      </c>
+      <c r="E574" t="n">
         <v>150</v>
-      </c>
-      <c r="D574" t="n">
-        <v>1</v>
-      </c>
-      <c r="E574" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="575">
@@ -10209,7 +10209,7 @@
         <v>4</v>
       </c>
       <c r="C575" t="n">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="D575" t="n">
         <v>1</v>
@@ -10226,13 +10226,13 @@
         <v>5</v>
       </c>
       <c r="C576" t="n">
+        <v>0</v>
+      </c>
+      <c r="D576" t="n">
+        <v>0</v>
+      </c>
+      <c r="E576" t="n">
         <v>150</v>
-      </c>
-      <c r="D576" t="n">
-        <v>1</v>
-      </c>
-      <c r="E576" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="577">
@@ -10243,7 +10243,7 @@
         <v>6</v>
       </c>
       <c r="C577" t="n">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="D577" t="n">
         <v>1</v>
@@ -10260,13 +10260,13 @@
         <v>7</v>
       </c>
       <c r="C578" t="n">
+        <v>0</v>
+      </c>
+      <c r="D578" t="n">
+        <v>0</v>
+      </c>
+      <c r="E578" t="n">
         <v>150</v>
-      </c>
-      <c r="D578" t="n">
-        <v>1</v>
-      </c>
-      <c r="E578" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="579">
@@ -10277,7 +10277,7 @@
         <v>8</v>
       </c>
       <c r="C579" t="n">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="D579" t="n">
         <v>1</v>
@@ -10294,13 +10294,13 @@
         <v>9</v>
       </c>
       <c r="C580" t="n">
+        <v>0</v>
+      </c>
+      <c r="D580" t="n">
+        <v>0</v>
+      </c>
+      <c r="E580" t="n">
         <v>150</v>
-      </c>
-      <c r="D580" t="n">
-        <v>1</v>
-      </c>
-      <c r="E580" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="581">
@@ -10311,7 +10311,7 @@
         <v>10</v>
       </c>
       <c r="C581" t="n">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="D581" t="n">
         <v>1</v>
@@ -10328,13 +10328,13 @@
         <v>11</v>
       </c>
       <c r="C582" t="n">
+        <v>0</v>
+      </c>
+      <c r="D582" t="n">
+        <v>0</v>
+      </c>
+      <c r="E582" t="n">
         <v>150</v>
-      </c>
-      <c r="D582" t="n">
-        <v>1</v>
-      </c>
-      <c r="E582" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="583">
@@ -10345,7 +10345,7 @@
         <v>12</v>
       </c>
       <c r="C583" t="n">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="D583" t="n">
         <v>1</v>
@@ -10362,13 +10362,13 @@
         <v>13</v>
       </c>
       <c r="C584" t="n">
+        <v>0</v>
+      </c>
+      <c r="D584" t="n">
+        <v>0</v>
+      </c>
+      <c r="E584" t="n">
         <v>150</v>
-      </c>
-      <c r="D584" t="n">
-        <v>1</v>
-      </c>
-      <c r="E584" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="585">
@@ -10379,7 +10379,7 @@
         <v>14</v>
       </c>
       <c r="C585" t="n">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="D585" t="n">
         <v>1</v>
@@ -10396,13 +10396,13 @@
         <v>15</v>
       </c>
       <c r="C586" t="n">
+        <v>0</v>
+      </c>
+      <c r="D586" t="n">
+        <v>0</v>
+      </c>
+      <c r="E586" t="n">
         <v>150</v>
-      </c>
-      <c r="D586" t="n">
-        <v>1</v>
-      </c>
-      <c r="E586" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="587">
@@ -10413,7 +10413,7 @@
         <v>16</v>
       </c>
       <c r="C587" t="n">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="D587" t="n">
         <v>1</v>
@@ -10430,13 +10430,13 @@
         <v>17</v>
       </c>
       <c r="C588" t="n">
-        <v>160</v>
+        <v>0</v>
       </c>
       <c r="D588" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E588" t="n">
-        <v>0</v>
+        <v>150</v>
       </c>
     </row>
     <row r="589">
@@ -10447,13 +10447,13 @@
         <v>18</v>
       </c>
       <c r="C589" t="n">
-        <v>140</v>
+        <v>300</v>
       </c>
       <c r="D589" t="n">
         <v>1</v>
       </c>
       <c r="E589" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="590">
@@ -10464,13 +10464,13 @@
         <v>19</v>
       </c>
       <c r="C590" t="n">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="D590" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E590" t="n">
-        <v>0</v>
+        <v>150</v>
       </c>
     </row>
     <row r="591">
@@ -10481,13 +10481,13 @@
         <v>20</v>
       </c>
       <c r="C591" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="D591" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E591" t="n">
-        <v>150</v>
+        <v>0</v>
       </c>
     </row>
     <row r="592">
@@ -10498,13 +10498,13 @@
         <v>21</v>
       </c>
       <c r="C592" t="n">
-        <v>307</v>
+        <v>0</v>
       </c>
       <c r="D592" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E592" t="n">
-        <v>0</v>
+        <v>150</v>
       </c>
     </row>
     <row r="593">
@@ -10515,13 +10515,13 @@
         <v>22</v>
       </c>
       <c r="C593" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="D593" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E593" t="n">
-        <v>157</v>
+        <v>0</v>
       </c>
     </row>
     <row r="594">
@@ -10532,13 +10532,13 @@
         <v>23</v>
       </c>
       <c r="C594" t="n">
-        <v>293</v>
+        <v>0</v>
       </c>
       <c r="D594" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E594" t="n">
-        <v>7</v>
+        <v>150</v>
       </c>
     </row>
     <row r="595">
@@ -10549,13 +10549,13 @@
         <v>24</v>
       </c>
       <c r="C595" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="D595" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E595" t="n">
-        <v>150</v>
+        <v>0</v>
       </c>
     </row>
     <row r="596">
@@ -10566,13 +10566,13 @@
         <v>25</v>
       </c>
       <c r="C596" t="n">
-        <v>450</v>
+        <v>0</v>
       </c>
       <c r="D596" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E596" t="n">
-        <v>0</v>
+        <v>150</v>
       </c>
     </row>
     <row r="597">
@@ -10583,13 +10583,13 @@
         <v>26</v>
       </c>
       <c r="C597" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="D597" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E597" t="n">
-        <v>300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="598">
@@ -10600,10 +10600,10 @@
         <v>27</v>
       </c>
       <c r="C598" t="n">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D598" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E598" t="n">
         <v>150</v>
@@ -10617,13 +10617,13 @@
         <v>28</v>
       </c>
       <c r="C599" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="D599" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E599" t="n">
-        <v>150</v>
+        <v>0</v>
       </c>
     </row>
     <row r="600">
@@ -10634,13 +10634,13 @@
         <v>29</v>
       </c>
       <c r="C600" t="n">
+        <v>0</v>
+      </c>
+      <c r="D600" t="n">
+        <v>0</v>
+      </c>
+      <c r="E600" t="n">
         <v>150</v>
-      </c>
-      <c r="D600" t="n">
-        <v>1</v>
-      </c>
-      <c r="E600" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="601">

</xml_diff>